<commit_message>
added values of Multi-Instance-2-sinks
</commit_message>
<xml_diff>
--- a/Observations.xlsx
+++ b/Observations.xlsx
@@ -1,29 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/balajibv/Desktop/Capstone project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/balajibv/Desktop/Capstone project/capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F3564D-C6A4-9646-ADDF-D3D8138E9F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5921FD6E-F791-3442-AA93-D2CA8D17BAD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{DAC0453D-D72E-AB4E-ACEF-62E600A84B55}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14040" xr2:uid="{DAC0453D-D72E-AB4E-ACEF-62E600A84B55}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$78</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$79</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$77:$D$77</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$78:$D$78</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$79:$D$79</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,6 +29,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -43,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="23">
   <si>
     <t>RECEPTION RATIO</t>
   </si>
@@ -96,7 +90,22 @@
     <t>PDR COMPARISION ( % )</t>
   </si>
   <si>
-    <t>ß</t>
+    <t>MULTIPLE INSTANCE + MULTIPLE SINK(OF0 + MRHOF) 38 + 2 Nodes</t>
+  </si>
+  <si>
+    <t>MULTIPLE INSTANCE + MULTIPLE SINK(OF0 + MRHOF) 38 + 3 Nodes</t>
+  </si>
+  <si>
+    <t>Multi-Instance &amp; Multi-Sink (3)</t>
+  </si>
+  <si>
+    <t>Multi-Instance &amp; Multi-Sink (2)</t>
+  </si>
+  <si>
+    <t>Multi-Instance &amp; Multi-Sink(3)</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -139,11 +148,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -152,6 +158,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,7 +376,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Multi-Instance &amp; Multi-Sink</c:v>
+                  <c:v>Multi-Instance &amp; Multi-Sink (3)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -444,6 +463,105 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-07B9-264A-98D2-C58D4AB877E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Multi-Instance &amp; Multi-Sink (2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$B$27:$F$28</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="5"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>100%</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>95%</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>90%</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>85%</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>80%</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>RECEPTION RATIO</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$31:$F$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>461</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>516</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>596</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>701</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>756</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-57F2-2D4C-BA89-A480545A973B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -839,7 +957,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Multi-Instance &amp; Multi-Sink</c:v>
+                  <c:v>Multi-Instance &amp; Multi-Sink (3)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -926,6 +1044,105 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-CB6F-7E4C-A757-A237A981FBA2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$48</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Multi-Instance &amp; Multi-Sink (2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$B$44:$F$45</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="5"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>100%</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>95%</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>90%</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>85%</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>80%</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>RECEPTION RATIO</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$48:$F$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>110.3441</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>109.7901</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>119.13890000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>126.30229</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>134.26320000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A227-F049-8CE1-EE25A9D8B8E7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1321,7 +1538,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Multi-Instance &amp; Multi-Sink</c:v>
+                  <c:v>Multi-Instance &amp; Multi-Sink(3)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1408,6 +1625,105 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-CC73-0B45-9EBD-7B054C6509DD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$64</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Multi-Instance &amp; Multi-Sink (2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$B$60:$F$61</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="5"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>100%</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>95%</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>90%</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>85%</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>80%</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>RECEPTION RATIO</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$64:$F$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>149846.35060000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>149856.54337</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>149890.53409999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>149928.01509999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>149925.86189999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BED7-014A-8881-B4BA9D5EEE29}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1479,6 +1795,7 @@
         <c:axId val="1049328719"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="149820"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1796,7 +2113,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Multi-Instance &amp; Multi-Sink</c:v>
+                  <c:v>Multi-Instance &amp; Multi-Sink(3)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1877,6 +2194,99 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6917-1A4A-AF76-CFEEBF2528B4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$80</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Multi-Instance &amp; Multi-Sink (2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$77:$F$77</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$80:$F$80</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>99.934000000000012</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>99.988333333333344</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>99.871403333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>99.988333333333344</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ECD7-0442-83ED-738D7DC88A15}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1948,7 +2358,7 @@
         <c:axId val="1455608096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="98"/>
+          <c:min val="99"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -5725,10 +6135,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FE58C2-2067-D844-87E0-17C046724E4B}">
-  <dimension ref="A1:I79"/>
+  <dimension ref="A1:V80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E80" sqref="E80"/>
+    <sheetView tabSelected="1" topLeftCell="E5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5738,54 +6148,83 @@
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
     <col min="4" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" customWidth="1"/>
+    <col min="14" max="14" width="29" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" customWidth="1"/>
+    <col min="16" max="16" width="13.5" customWidth="1"/>
+    <col min="17" max="17" width="12.83203125" customWidth="1"/>
+    <col min="18" max="18" width="13.33203125" customWidth="1"/>
+    <col min="19" max="19" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="1" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="N2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>0.95</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>0.9</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>0.85</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="N3" s="6"/>
+      <c r="O3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B4">
@@ -5803,9 +6242,28 @@
       <c r="F4">
         <v>99.569500000000005</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="N4" s="6"/>
+      <c r="O4" s="7">
+        <v>1</v>
+      </c>
+      <c r="P4" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="R4" s="7">
+        <v>0.85</v>
+      </c>
+      <c r="S4" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5">
@@ -5823,9 +6281,30 @@
       <c r="F5">
         <v>98.334900000000005</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="N5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="O5" s="4">
+        <v>99.895200000000003</v>
+      </c>
+      <c r="P5" s="4">
+        <v>100</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>99.965000000000003</v>
+      </c>
+      <c r="R5" s="4">
+        <v>99.9298</v>
+      </c>
+      <c r="S5" s="4">
+        <v>99.965000000000003</v>
+      </c>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B6">
@@ -5843,9 +6322,30 @@
       <c r="F6">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="N6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="O6" s="4">
+        <v>99.906800000000004</v>
+      </c>
+      <c r="P6" s="4">
+        <v>100</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>100</v>
+      </c>
+      <c r="R6" s="4">
+        <v>99.906710000000004</v>
+      </c>
+      <c r="S6" s="4">
+        <v>100</v>
+      </c>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B7">
@@ -5868,9 +6368,30 @@
         <f>AVERAGE(F4:F6)</f>
         <v>99.30146666666667</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="N7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7" s="4">
+        <v>100</v>
+      </c>
+      <c r="P7" s="4">
+        <v>100</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>100</v>
+      </c>
+      <c r="R7" s="4">
+        <v>99.777699999999996</v>
+      </c>
+      <c r="S7" s="4">
+        <v>100</v>
+      </c>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -5888,9 +6409,35 @@
       <c r="F8">
         <v>143.0651</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="N8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="O8" s="4">
+        <f>AVERAGE(O5:O7)</f>
+        <v>99.934000000000012</v>
+      </c>
+      <c r="P8" s="4">
+        <f>AVERAGE(P5:P7)</f>
+        <v>100</v>
+      </c>
+      <c r="Q8" s="4">
+        <f>AVERAGE(Q5:Q7)</f>
+        <v>99.988333333333344</v>
+      </c>
+      <c r="R8" s="4">
+        <f>AVERAGE(R5:R7)</f>
+        <v>99.871403333333333</v>
+      </c>
+      <c r="S8" s="4">
+        <f>AVERAGE(S5:S7)</f>
+        <v>99.988333333333344</v>
+      </c>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -5908,9 +6455,30 @@
       <c r="F9">
         <v>1016</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="N9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O9" s="4">
+        <v>110.3441</v>
+      </c>
+      <c r="P9" s="4">
+        <v>109.7901</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>119.13890000000001</v>
+      </c>
+      <c r="R9" s="4">
+        <v>126.30229</v>
+      </c>
+      <c r="S9" s="4">
+        <v>134.26320000000001</v>
+      </c>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B10">
@@ -5928,58 +6496,100 @@
       <c r="F10">
         <v>150167.91339999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O10" s="4">
+        <v>461</v>
+      </c>
+      <c r="P10" s="4">
+        <v>516</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>596</v>
+      </c>
+      <c r="R10" s="4">
+        <v>701</v>
+      </c>
+      <c r="S10" s="4">
+        <v>756</v>
+      </c>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="1" t="s">
+      <c r="N11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O11" s="4">
+        <v>149846.35060000001</v>
+      </c>
+      <c r="P11" s="4">
+        <v>149856.54337</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>149890.53409999999</v>
+      </c>
+      <c r="R11" s="4">
+        <v>149928.01509999999</v>
+      </c>
+      <c r="S11" s="4">
+        <v>149925.86189999999</v>
+      </c>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3">
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2">
         <v>1</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>0.95</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>0.9</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>0.85</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <v>0.8</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B16">
@@ -5998,8 +6608,8 @@
         <v>99.965000000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B17">
@@ -6018,8 +6628,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B18">
@@ -6038,8 +6648,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B19">
@@ -6063,8 +6673,8 @@
         <v>99.988333333333344</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B20">
@@ -6083,8 +6693,8 @@
         <v>121.8613</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B21">
@@ -6103,8 +6713,8 @@
         <v>621</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B22">
@@ -6123,57 +6733,57 @@
         <v>149879.2727</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="1" t="s">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="3">
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2">
         <v>1</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="2">
         <v>0.95</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2">
         <v>0.9</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <v>0.85</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="2">
         <v>0.8</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B29">
@@ -6197,9 +6807,9 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>10</v>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B30">
         <f>B21</f>
@@ -6222,64 +6832,86 @@
         <v>621</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31">
+        <f>O10</f>
+        <v>461</v>
+      </c>
+      <c r="C31">
+        <f>P10</f>
+        <v>516</v>
+      </c>
+      <c r="D31">
+        <f>Q10</f>
+        <v>596</v>
+      </c>
+      <c r="E31">
+        <f>R10</f>
+        <v>701</v>
+      </c>
+      <c r="F31">
+        <f>S10</f>
+        <v>756</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
+      <c r="A33" s="1"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
+      <c r="A34" s="1"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
-      <c r="B44" s="1" t="s">
+      <c r="A44" s="1"/>
+      <c r="B44" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
-      <c r="B45" s="3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="2">
         <v>1</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="2">
         <v>0.95</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="2">
         <v>0.9</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="2">
         <v>0.85</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F45" s="2">
         <v>0.8</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B46">
@@ -6304,22 +6936,22 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B47" s="5">
+      <c r="A47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="4">
         <f>B20</f>
         <v>110.86969999999999</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C47" s="4">
         <f>C20</f>
         <v>113.6323</v>
       </c>
-      <c r="D47" s="5">
+      <c r="D47" s="4">
         <f>D20</f>
         <v>112.3976</v>
       </c>
-      <c r="E47" s="5">
+      <c r="E47" s="4">
         <f>E20</f>
         <v>124.0538</v>
       </c>
@@ -6328,52 +6960,77 @@
         <v>121.8613</v>
       </c>
     </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48">
+        <f>O9</f>
+        <v>110.3441</v>
+      </c>
+      <c r="C48">
+        <f>P9</f>
+        <v>109.7901</v>
+      </c>
+      <c r="D48">
+        <f>Q9</f>
+        <v>119.13890000000001</v>
+      </c>
+      <c r="E48">
+        <f>R9</f>
+        <v>126.30229</v>
+      </c>
+      <c r="F48">
+        <f>S9</f>
+        <v>134.26320000000001</v>
+      </c>
+    </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-      <c r="I59" s="1"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="2"/>
-      <c r="B60" s="1" t="s">
+      <c r="A60" s="1"/>
+      <c r="B60" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" s="2"/>
-      <c r="B61" s="3">
+      <c r="A61" s="1"/>
+      <c r="B61" s="2">
         <v>1</v>
       </c>
-      <c r="C61" s="3">
+      <c r="C61" s="2">
         <v>0.95</v>
       </c>
-      <c r="D61" s="3">
+      <c r="D61" s="2">
         <v>0.9</v>
       </c>
-      <c r="E61" s="3">
+      <c r="E61" s="2">
         <v>0.85</v>
       </c>
-      <c r="F61" s="3">
+      <c r="F61" s="2">
         <v>0.8</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B62">
@@ -6398,8 +7055,8 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
-        <v>10</v>
+      <c r="A63" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B63">
         <f>B22</f>
@@ -6422,52 +7079,77 @@
         <v>149879.2727</v>
       </c>
     </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>20</v>
+      </c>
+      <c r="B64">
+        <f>O11</f>
+        <v>149846.35060000001</v>
+      </c>
+      <c r="C64">
+        <f>P11</f>
+        <v>149856.54337</v>
+      </c>
+      <c r="D64">
+        <f>Q11</f>
+        <v>149890.53409999999</v>
+      </c>
+      <c r="E64">
+        <f>R11</f>
+        <v>149928.01509999999</v>
+      </c>
+      <c r="F64">
+        <f>S11</f>
+        <v>149925.86189999999</v>
+      </c>
+    </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
-      <c r="H75" s="1"/>
-      <c r="I75" s="1"/>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A76" s="2"/>
-      <c r="B76" s="1" t="s">
+      <c r="A76" s="1"/>
+      <c r="B76" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
-      <c r="G76" s="2"/>
-      <c r="H76" s="2"/>
-      <c r="I76" s="2"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A77" s="2"/>
-      <c r="B77" s="3">
+      <c r="A77" s="1"/>
+      <c r="B77" s="2">
         <v>1</v>
       </c>
-      <c r="C77" s="3">
+      <c r="C77" s="2">
         <v>0.95</v>
       </c>
-      <c r="D77" s="3">
+      <c r="D77" s="2">
         <v>0.9</v>
       </c>
-      <c r="E77" s="3">
+      <c r="E77" s="2">
         <v>0.85</v>
       </c>
-      <c r="F77" s="3">
+      <c r="F77" s="2">
         <v>0.8</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A78" s="4" t="s">
+      <c r="A78" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B78">
@@ -6492,8 +7174,8 @@
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A79" s="2" t="s">
-        <v>10</v>
+      <c r="A79" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B79">
         <f>B19</f>
@@ -6516,13 +7198,35 @@
         <v>99.988333333333344</v>
       </c>
     </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>20</v>
+      </c>
+      <c r="B80">
+        <f>O8</f>
+        <v>99.934000000000012</v>
+      </c>
+      <c r="C80">
+        <f>P8</f>
+        <v>100</v>
+      </c>
+      <c r="D80">
+        <f>Q8</f>
+        <v>99.988333333333344</v>
+      </c>
+      <c r="E80">
+        <f>R8</f>
+        <v>99.871403333333333</v>
+      </c>
+      <c r="F80">
+        <f>S8</f>
+        <v>99.988333333333344</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="A43:I43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="A59:I59"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="A75:I75"/>
+  <mergeCells count="14">
+    <mergeCell ref="N2:V2"/>
+    <mergeCell ref="O3:S3"/>
     <mergeCell ref="B76:F76"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B2:F2"/>
@@ -6530,6 +7234,11 @@
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="A26:I26"/>
     <mergeCell ref="B27:F27"/>
+    <mergeCell ref="A43:I43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="A59:I59"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="A75:I75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -6555,46 +7264,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>0.85</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>0.7</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B4">
@@ -6611,7 +7320,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5">
@@ -6628,7 +7337,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B6">
@@ -6645,7 +7354,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B7">
@@ -6666,7 +7375,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -6683,7 +7392,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -6700,7 +7409,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B10">
@@ -6722,46 +7431,46 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="1" t="s">
+      <c r="A14" s="1"/>
+      <c r="B14" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2">
         <v>1</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>0.85</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>0.7</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B16">
@@ -6778,7 +7487,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B17">
@@ -6795,7 +7504,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B18">
@@ -6812,7 +7521,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B19">
@@ -6833,7 +7542,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B20">
@@ -6850,7 +7559,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B21">
@@ -6867,7 +7576,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B22">
@@ -6884,46 +7593,46 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="1" t="s">
+      <c r="A27" s="1"/>
+      <c r="B27" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2">
         <v>1</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="2">
         <v>0.85</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2">
         <v>0.7</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <v>0.5</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B29">
@@ -6944,7 +7653,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B30">
@@ -6965,58 +7674,58 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
+      <c r="A31" s="1"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
+      <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
+      <c r="A33" s="1"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
+      <c r="A34" s="1"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
-      <c r="B44" s="1" t="s">
+      <c r="A44" s="1"/>
+      <c r="B44" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
-      <c r="B45" s="3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="2">
         <v>1</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="2">
         <v>0.85</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="2">
         <v>0.7</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="2">
         <v>0.5</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B46">
@@ -7037,18 +7746,18 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B47" s="5">
+      <c r="B47" s="4">
         <f>B20</f>
         <v>110.86969999999999</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C47" s="4">
         <f>C20</f>
         <v>124.0538</v>
       </c>
-      <c r="D47" s="5">
+      <c r="D47" s="4">
         <f>D20</f>
         <v>130.90729999999999</v>
       </c>
@@ -7058,46 +7767,46 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="2"/>
-      <c r="B60" s="1" t="s">
+      <c r="A60" s="1"/>
+      <c r="B60" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="2"/>
-      <c r="B61" s="3">
+      <c r="A61" s="1"/>
+      <c r="B61" s="2">
         <v>1</v>
       </c>
-      <c r="C61" s="3">
+      <c r="C61" s="2">
         <v>0.85</v>
       </c>
-      <c r="D61" s="3">
+      <c r="D61" s="2">
         <v>0.7</v>
       </c>
-      <c r="E61" s="3">
+      <c r="E61" s="2">
         <v>0.5</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B62">
@@ -7118,7 +7827,7 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
+      <c r="A63" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B63">
@@ -7139,46 +7848,46 @@
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
-      <c r="H75" s="1"/>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="2"/>
-      <c r="B76" s="1" t="s">
+      <c r="A76" s="1"/>
+      <c r="B76" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="2"/>
-      <c r="G76" s="2"/>
-      <c r="H76" s="2"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" s="2"/>
-      <c r="B77" s="3">
+      <c r="A77" s="1"/>
+      <c r="B77" s="2">
         <v>1</v>
       </c>
-      <c r="C77" s="3">
+      <c r="C77" s="2">
         <v>0.85</v>
       </c>
-      <c r="D77" s="3">
+      <c r="D77" s="2">
         <v>0.7</v>
       </c>
-      <c r="E77" s="3">
+      <c r="E77" s="2">
         <v>0.5</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="4" t="s">
+      <c r="A78" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B78">
@@ -7199,7 +7908,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A79" s="2" t="s">
+      <c r="A79" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B79">
@@ -7221,11 +7930,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A43:H43"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="A59:H59"/>
-    <mergeCell ref="B60:E60"/>
-    <mergeCell ref="A75:H75"/>
     <mergeCell ref="B76:E76"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B2:E2"/>
@@ -7233,6 +7937,11 @@
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="A26:H26"/>
     <mergeCell ref="B27:E27"/>
+    <mergeCell ref="A43:H43"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="A59:H59"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="A75:H75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>